<commit_message>
updated test.py and added omnivore test data
</commit_message>
<xml_diff>
--- a/app/datasets/UkGovtHouseholdPurchases.xlsx
+++ b/app/datasets/UkGovtHouseholdPurchases.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/smithjj7_cardiff_ac_uk/Documents/Dissertation/GroceryEmissionTracker/app/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7FA1B5F7-6BC9-4112-9D4A-9879B9178D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{7FA1B5F7-6BC9-4112-9D4A-9879B9178D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E064932-2D99-419A-AD65-E9688637A34C}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="13005" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Household_quantity" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="604">
   <si>
     <t>Family Food Survey 2020/21: Notes</t>
   </si>
@@ -1130,9 +1143,6 @@
     <t>188</t>
   </si>
   <si>
-    <t>Beans canned</t>
-  </si>
-  <si>
     <t>18802</t>
   </si>
   <si>
@@ -1877,7 +1887,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;+&quot;#,##0;&quot;-&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2190,19 +2200,19 @@
   </cellStyleXfs>
   <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2233,7 +2243,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2491,12 +2501,12 @@
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="2"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal_final results02" xfId="6"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal_final results02" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2807,7 +2817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2882,25 +2892,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="J25" sqref="F25:J25"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1"/>
     <col min="6" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
@@ -8911,9 +8921,6 @@
       </c>
       <c r="B190" s="42"/>
       <c r="C190" s="42"/>
-      <c r="D190" s="42" t="s">
-        <v>357</v>
-      </c>
       <c r="E190" s="42"/>
       <c r="F190" s="43" t="s">
         <v>90</v>
@@ -8939,13 +8946,13 @@
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191" s="41" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B191" s="42"/>
       <c r="C191" s="42"/>
       <c r="D191" s="42"/>
       <c r="E191" s="42" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F191" s="43" t="s">
         <v>90</v>
@@ -8971,13 +8978,13 @@
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192" s="41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B192" s="42"/>
       <c r="C192" s="42"/>
       <c r="D192" s="42"/>
       <c r="E192" s="42" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F192" s="43" t="s">
         <v>90</v>
@@ -9012,7 +9019,7 @@
       <c r="B193" s="42"/>
       <c r="C193" s="42"/>
       <c r="D193" s="42" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E193" s="42"/>
       <c r="F193" s="43" t="s">
@@ -9044,7 +9051,7 @@
       <c r="B194" s="42"/>
       <c r="C194" s="42"/>
       <c r="D194" s="42" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E194" s="42"/>
       <c r="F194" s="43" t="s">
@@ -9074,7 +9081,7 @@
       <c r="B195" s="42"/>
       <c r="C195" s="42"/>
       <c r="D195" s="42" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E195" s="42"/>
       <c r="F195" s="43" t="s">
@@ -9105,12 +9112,12 @@
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196" s="41" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B196" s="42"/>
       <c r="C196" s="42"/>
       <c r="D196" s="42" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E196" s="42"/>
       <c r="F196" s="43" t="s">
@@ -9135,13 +9142,13 @@
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197" s="41" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B197" s="42"/>
       <c r="C197" s="42"/>
       <c r="D197" s="42"/>
       <c r="E197" s="42" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F197" s="43" t="s">
         <v>29</v>
@@ -9167,13 +9174,13 @@
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A198" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B198" s="42"/>
       <c r="C198" s="42"/>
       <c r="D198" s="42"/>
       <c r="E198" s="42" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F198" s="43" t="s">
         <v>29</v>
@@ -9204,7 +9211,7 @@
       <c r="B199" s="42"/>
       <c r="C199" s="42"/>
       <c r="D199" s="42" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E199" s="42"/>
       <c r="F199" s="43" t="s">
@@ -9236,7 +9243,7 @@
       <c r="B200" s="42"/>
       <c r="C200" s="42"/>
       <c r="D200" s="42" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E200" s="42"/>
       <c r="F200" s="43" t="s">
@@ -9261,12 +9268,12 @@
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201" s="41" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B201" s="42"/>
       <c r="C201" s="42"/>
       <c r="D201" s="42" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E201" s="42"/>
       <c r="F201" s="43" t="s">
@@ -9297,13 +9304,13 @@
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202" s="41" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B202" s="42"/>
       <c r="C202" s="42"/>
       <c r="D202" s="42"/>
       <c r="E202" s="42" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F202" s="43" t="s">
         <v>90</v>
@@ -9333,13 +9340,13 @@
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A203" s="41" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B203" s="42"/>
       <c r="C203" s="42"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F203" s="43" t="s">
         <v>90</v>
@@ -9370,7 +9377,7 @@
       <c r="B204" s="73"/>
       <c r="C204" s="73"/>
       <c r="D204" s="73" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E204" s="73"/>
       <c r="F204" s="57" t="s">
@@ -9397,10 +9404,10 @@
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A205" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="B205" s="68" t="s">
         <v>380</v>
-      </c>
-      <c r="B205" s="68" t="s">
-        <v>381</v>
       </c>
       <c r="C205" s="68"/>
       <c r="D205" s="68"/>
@@ -9429,11 +9436,11 @@
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A206" s="41" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B206" s="42"/>
       <c r="C206" s="42" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D206" s="42"/>
       <c r="E206" s="42"/>
@@ -9466,7 +9473,7 @@
       <c r="B207" s="42"/>
       <c r="C207" s="42"/>
       <c r="D207" s="42" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E207" s="42"/>
       <c r="F207" s="43" t="s">
@@ -9498,7 +9505,7 @@
       <c r="B208" s="42"/>
       <c r="C208" s="42"/>
       <c r="D208" s="42" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E208" s="42"/>
       <c r="F208" s="43" t="s">
@@ -9530,7 +9537,7 @@
       <c r="B209" s="42"/>
       <c r="C209" s="42"/>
       <c r="D209" s="42" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E209" s="42"/>
       <c r="F209" s="43" t="s">
@@ -9566,7 +9573,7 @@
       <c r="B210" s="42"/>
       <c r="C210" s="42"/>
       <c r="D210" s="42" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E210" s="42"/>
       <c r="F210" s="43" t="s">
@@ -9598,7 +9605,7 @@
       <c r="B211" s="42"/>
       <c r="C211" s="42"/>
       <c r="D211" s="42" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E211" s="42"/>
       <c r="F211" s="43" t="s">
@@ -9630,7 +9637,7 @@
       <c r="B212" s="42"/>
       <c r="C212" s="42"/>
       <c r="D212" s="42" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E212" s="42"/>
       <c r="F212" s="43" t="s">
@@ -9666,7 +9673,7 @@
       <c r="B213" s="42"/>
       <c r="C213" s="42"/>
       <c r="D213" s="42" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E213" s="42"/>
       <c r="F213" s="43" t="s">
@@ -9702,7 +9709,7 @@
       <c r="B214" s="42"/>
       <c r="C214" s="42"/>
       <c r="D214" s="42" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E214" s="42"/>
       <c r="F214" s="43" t="s">
@@ -9734,7 +9741,7 @@
       <c r="B215" s="42"/>
       <c r="C215" s="42"/>
       <c r="D215" s="42" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E215" s="42"/>
       <c r="F215" s="43" t="s">
@@ -9766,7 +9773,7 @@
       <c r="B216" s="42"/>
       <c r="C216" s="42"/>
       <c r="D216" s="42" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E216" s="42"/>
       <c r="F216" s="43" t="s">
@@ -9793,11 +9800,11 @@
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B217" s="42"/>
       <c r="C217" s="42" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D217" s="42"/>
       <c r="E217" s="42"/>
@@ -9832,7 +9839,7 @@
       <c r="B218" s="42"/>
       <c r="C218" s="42"/>
       <c r="D218" s="42" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E218" s="42"/>
       <c r="F218" s="43" t="s">
@@ -9862,7 +9869,7 @@
       <c r="B219" s="42"/>
       <c r="C219" s="42"/>
       <c r="D219" s="42" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E219" s="42"/>
       <c r="F219" s="43" t="s">
@@ -9894,7 +9901,7 @@
       <c r="B220" s="42"/>
       <c r="C220" s="42"/>
       <c r="D220" s="42" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E220" s="42"/>
       <c r="F220" s="43" t="s">
@@ -9930,7 +9937,7 @@
       <c r="B221" s="42"/>
       <c r="C221" s="42"/>
       <c r="D221" s="42" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E221" s="42"/>
       <c r="F221" s="43" t="s">
@@ -9959,12 +9966,12 @@
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B222" s="42"/>
       <c r="C222" s="42"/>
       <c r="D222" s="42" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E222" s="42"/>
       <c r="F222" s="43" t="s">
@@ -9995,13 +10002,13 @@
     </row>
     <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223" s="41" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B223" s="42"/>
       <c r="C223" s="42"/>
       <c r="D223" s="42"/>
       <c r="E223" s="42" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F223" s="43" t="s">
         <v>90</v>
@@ -10031,13 +10038,13 @@
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224" s="41" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B224" s="42"/>
       <c r="C224" s="42"/>
       <c r="D224" s="42"/>
       <c r="E224" s="42" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F224" s="43" t="s">
         <v>90</v>
@@ -10072,7 +10079,7 @@
       <c r="B225" s="73"/>
       <c r="C225" s="73"/>
       <c r="D225" s="73" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E225" s="73"/>
       <c r="F225" s="57" t="s">
@@ -10099,11 +10106,11 @@
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226" s="30" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B226" s="68"/>
       <c r="C226" s="68" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D226" s="68"/>
       <c r="E226" s="68"/>
@@ -10133,10 +10140,10 @@
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="B227" s="42" t="s">
         <v>409</v>
-      </c>
-      <c r="B227" s="42" t="s">
-        <v>410</v>
       </c>
       <c r="C227" s="42"/>
       <c r="D227" s="42"/>
@@ -10174,7 +10181,7 @@
       <c r="B228" s="42"/>
       <c r="C228" s="42"/>
       <c r="D228" s="42" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E228" s="42"/>
       <c r="F228" s="43" t="s">
@@ -10208,7 +10215,7 @@
       <c r="B229" s="42"/>
       <c r="C229" s="42"/>
       <c r="D229" s="42" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E229" s="42"/>
       <c r="F229" s="43" t="s">
@@ -10244,7 +10251,7 @@
       <c r="B230" s="42"/>
       <c r="C230" s="42"/>
       <c r="D230" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E230" s="42"/>
       <c r="F230" s="43" t="s">
@@ -10276,7 +10283,7 @@
       <c r="B231" s="42"/>
       <c r="C231" s="42"/>
       <c r="D231" s="42" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E231" s="42"/>
       <c r="F231" s="43" t="s">
@@ -10301,10 +10308,10 @@
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232" s="41" t="s">
+        <v>414</v>
+      </c>
+      <c r="B232" s="42" t="s">
         <v>415</v>
-      </c>
-      <c r="B232" s="42" t="s">
-        <v>416</v>
       </c>
       <c r="C232" s="42"/>
       <c r="D232" s="42"/>
@@ -10338,7 +10345,7 @@
       <c r="B233" s="42"/>
       <c r="C233" s="42"/>
       <c r="D233" s="42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E233" s="42"/>
       <c r="F233" s="43" t="s">
@@ -10370,7 +10377,7 @@
       <c r="B234" s="42"/>
       <c r="C234" s="42"/>
       <c r="D234" s="42" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E234" s="42"/>
       <c r="F234" s="43" t="s">
@@ -10397,12 +10404,12 @@
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235" s="41" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B235" s="42"/>
       <c r="C235" s="42"/>
       <c r="D235" s="42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E235" s="42"/>
       <c r="F235" s="43" t="s">
@@ -10429,13 +10436,13 @@
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236" s="41" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B236" s="42"/>
       <c r="C236" s="42"/>
       <c r="D236" s="42"/>
       <c r="E236" s="42" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F236" s="43" t="s">
         <v>90</v>
@@ -10465,13 +10472,13 @@
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237" s="41" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B237" s="42"/>
       <c r="C237" s="42"/>
       <c r="D237" s="42"/>
       <c r="E237" s="42" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F237" s="43" t="s">
         <v>90</v>
@@ -10495,13 +10502,13 @@
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238" s="41" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B238" s="42"/>
       <c r="C238" s="42"/>
       <c r="D238" s="42"/>
       <c r="E238" s="42" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F238" s="43" t="s">
         <v>90</v>
@@ -10527,13 +10534,13 @@
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239" s="41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B239" s="42"/>
       <c r="C239" s="42"/>
       <c r="D239" s="42"/>
       <c r="E239" s="42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F239" s="43" t="s">
         <v>90</v>
@@ -10557,13 +10564,13 @@
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240" s="41" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B240" s="42"/>
       <c r="C240" s="42"/>
       <c r="D240" s="42"/>
       <c r="E240" s="42" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F240" s="43" t="s">
         <v>90</v>
@@ -10593,13 +10600,13 @@
     </row>
     <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241" s="41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B241" s="42"/>
       <c r="C241" s="42"/>
       <c r="D241" s="42"/>
       <c r="E241" s="42" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F241" s="43" t="s">
         <v>90</v>
@@ -10629,13 +10636,13 @@
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242" s="41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B242" s="42"/>
       <c r="C242" s="42"/>
       <c r="D242" s="42"/>
       <c r="E242" s="42" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F242" s="43" t="s">
         <v>90</v>
@@ -10659,13 +10666,13 @@
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243" s="79" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B243" s="73"/>
       <c r="C243" s="73"/>
       <c r="D243" s="73"/>
       <c r="E243" s="73" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F243" s="80" t="s">
         <v>90</v>
@@ -10693,7 +10700,7 @@
       </c>
       <c r="B244" s="86"/>
       <c r="C244" s="86" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D244" s="86"/>
       <c r="E244" s="86"/>
@@ -10721,11 +10728,11 @@
     </row>
     <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245" s="30" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B245" s="63"/>
       <c r="C245" s="63" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D245" s="63"/>
       <c r="E245" s="63"/>
@@ -10756,7 +10763,7 @@
         <v>267</v>
       </c>
       <c r="D246" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F246" s="80" t="s">
         <v>90</v>
@@ -10784,12 +10791,12 @@
     </row>
     <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B247" s="105"/>
       <c r="C247" s="105"/>
       <c r="D247" s="105" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E247" s="105"/>
       <c r="F247" s="106" t="s">
@@ -10816,13 +10823,13 @@
     </row>
     <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248" s="79" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B248" s="94"/>
       <c r="C248" s="94"/>
       <c r="D248" s="94"/>
       <c r="E248" s="94" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F248" s="80" t="s">
         <v>90</v>
@@ -10848,13 +10855,13 @@
     </row>
     <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249" s="55" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B249" s="73"/>
       <c r="C249" s="73"/>
       <c r="D249" s="73"/>
       <c r="E249" s="73" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F249" s="57" t="s">
         <v>90</v>
@@ -10878,11 +10885,11 @@
     </row>
     <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250" s="30" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B250" s="31"/>
       <c r="C250" s="31" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D250" s="31"/>
       <c r="E250" s="31"/>
@@ -10913,7 +10920,7 @@
         <v>271</v>
       </c>
       <c r="D251" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F251" s="80" t="s">
         <v>90</v>
@@ -10939,12 +10946,12 @@
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252" s="41" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B252" s="42"/>
       <c r="C252" s="42"/>
       <c r="D252" s="42" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E252" s="42"/>
       <c r="F252" s="43" t="s">
@@ -10971,13 +10978,13 @@
     </row>
     <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253" s="41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B253" s="42"/>
       <c r="C253" s="42"/>
       <c r="D253" s="42"/>
       <c r="E253" s="42" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F253" s="43" t="s">
         <v>90</v>
@@ -11003,13 +11010,13 @@
     </row>
     <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254" s="79" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B254" s="94"/>
       <c r="C254" s="94"/>
       <c r="D254" s="94"/>
       <c r="E254" s="94" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F254" s="80" t="s">
         <v>90</v>
@@ -11040,7 +11047,7 @@
       <c r="B255" s="73"/>
       <c r="C255" s="73"/>
       <c r="D255" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E255" s="73"/>
       <c r="F255" s="57" t="s">
@@ -11067,11 +11074,11 @@
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256" s="30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B256" s="31"/>
       <c r="C256" s="31" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D256" s="31"/>
       <c r="E256" s="31"/>
@@ -11106,7 +11113,7 @@
       <c r="B257" s="42"/>
       <c r="C257" s="42"/>
       <c r="D257" s="42" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E257" s="42"/>
       <c r="F257" s="43" t="s">
@@ -11133,12 +11140,12 @@
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258" s="41" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B258" s="42"/>
       <c r="C258" s="42"/>
       <c r="D258" s="42" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E258" s="111"/>
       <c r="F258" s="43" t="s">
@@ -11165,13 +11172,13 @@
     </row>
     <row r="259" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A259" s="41" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B259" s="42"/>
       <c r="C259" s="42"/>
       <c r="D259" s="42"/>
       <c r="E259" s="42" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F259" s="43" t="s">
         <v>90</v>
@@ -11197,13 +11204,13 @@
     </row>
     <row r="260" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A260" s="41" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B260" s="42"/>
       <c r="C260" s="42"/>
       <c r="D260" s="42"/>
       <c r="E260" s="42" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F260" s="43" t="s">
         <v>90</v>
@@ -11229,13 +11236,13 @@
     </row>
     <row r="261" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A261" s="41" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B261" s="42"/>
       <c r="C261" s="42"/>
       <c r="D261" s="42"/>
       <c r="E261" s="42" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F261" s="43" t="s">
         <v>90</v>
@@ -11261,13 +11268,13 @@
     </row>
     <row r="262" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A262" s="41" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B262" s="42"/>
       <c r="C262" s="42"/>
       <c r="D262" s="42"/>
       <c r="E262" s="42" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F262" s="43" t="s">
         <v>90</v>
@@ -11297,12 +11304,12 @@
     </row>
     <row r="263" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A263" s="41" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B263" s="42"/>
       <c r="C263" s="42"/>
       <c r="D263" s="42" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E263" s="42"/>
       <c r="F263" s="43" t="s">
@@ -11329,13 +11336,13 @@
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264" s="41" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B264" s="42"/>
       <c r="C264" s="42"/>
       <c r="D264" s="42"/>
       <c r="E264" s="42" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F264" s="43" t="s">
         <v>90</v>
@@ -11361,13 +11368,13 @@
     </row>
     <row r="265" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A265" s="41" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B265" s="42"/>
       <c r="C265" s="42"/>
       <c r="D265" s="42"/>
       <c r="E265" s="42" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F265" s="43" t="s">
         <v>90</v>
@@ -11396,7 +11403,7 @@
       <c r="B266" s="42"/>
       <c r="C266" s="42"/>
       <c r="D266" s="42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E266" s="42"/>
       <c r="F266" s="43" t="s">
@@ -11423,12 +11430,12 @@
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A267" s="41" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B267" s="42"/>
       <c r="C267" s="42"/>
       <c r="D267" s="42" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E267" s="42"/>
       <c r="F267" s="43" t="s">
@@ -11455,13 +11462,13 @@
     </row>
     <row r="268" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A268" s="41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B268" s="42"/>
       <c r="C268" s="42"/>
       <c r="D268" s="42"/>
       <c r="E268" s="42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F268" s="43" t="s">
         <v>90</v>
@@ -11485,13 +11492,13 @@
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A269" s="41" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B269" s="42"/>
       <c r="C269" s="42"/>
       <c r="D269" s="42"/>
       <c r="E269" s="42" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F269" s="43" t="s">
         <v>90</v>
@@ -11519,13 +11526,13 @@
     </row>
     <row r="270" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A270" s="41" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B270" s="42"/>
       <c r="C270" s="42"/>
       <c r="D270" s="42"/>
       <c r="E270" s="42" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F270" s="43" t="s">
         <v>90</v>
@@ -11560,7 +11567,7 @@
       <c r="B271" s="42"/>
       <c r="C271" s="42"/>
       <c r="D271" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E271" s="42"/>
       <c r="F271" s="43" t="s">
@@ -11590,7 +11597,7 @@
       <c r="B272" s="42"/>
       <c r="C272" s="42"/>
       <c r="D272" s="42" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E272" s="42"/>
       <c r="F272" s="43" t="s">
@@ -11622,7 +11629,7 @@
       <c r="B273" s="42"/>
       <c r="C273" s="42"/>
       <c r="D273" s="42" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E273" s="42"/>
       <c r="F273" s="43" t="s">
@@ -11649,12 +11656,12 @@
     </row>
     <row r="274" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A274" s="41" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B274" s="42"/>
       <c r="C274" s="42"/>
       <c r="D274" s="42" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E274" s="42"/>
       <c r="F274" s="43" t="s">
@@ -11685,13 +11692,13 @@
     </row>
     <row r="275" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A275" s="41" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B275" s="42"/>
       <c r="C275" s="42"/>
       <c r="D275" s="42"/>
       <c r="E275" s="42" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F275" s="43" t="s">
         <v>90</v>
@@ -11715,13 +11722,13 @@
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A276" s="41" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B276" s="42"/>
       <c r="C276" s="42"/>
       <c r="D276" s="42"/>
       <c r="E276" s="42" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F276" s="43" t="s">
         <v>90</v>
@@ -11751,13 +11758,13 @@
     </row>
     <row r="277" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A277" s="41" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B277" s="42"/>
       <c r="C277" s="42"/>
       <c r="D277" s="42"/>
       <c r="E277" s="42" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F277" s="43" t="s">
         <v>90</v>
@@ -11783,12 +11790,12 @@
     </row>
     <row r="278" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A278" s="41" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B278" s="42"/>
       <c r="C278" s="42"/>
       <c r="D278" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E278" s="42"/>
       <c r="F278" s="43" t="s">
@@ -11815,13 +11822,13 @@
     </row>
     <row r="279" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A279" s="41" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B279" s="42"/>
       <c r="C279" s="42"/>
       <c r="D279" s="42"/>
       <c r="E279" s="42" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F279" s="43" t="s">
         <v>90</v>
@@ -11847,13 +11854,13 @@
     </row>
     <row r="280" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A280" s="41" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B280" s="42"/>
       <c r="C280" s="42"/>
       <c r="D280" s="42"/>
       <c r="E280" s="42" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F280" s="43" t="s">
         <v>90</v>
@@ -11879,12 +11886,12 @@
     </row>
     <row r="281" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A281" s="41" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B281" s="42"/>
       <c r="C281" s="42"/>
       <c r="D281" s="42" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E281" s="42"/>
       <c r="F281" s="43" t="s">
@@ -11915,13 +11922,13 @@
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A282" s="41" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B282" s="42"/>
       <c r="C282" s="42"/>
       <c r="D282" s="42"/>
       <c r="E282" s="42" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F282" s="43" t="s">
         <v>90</v>
@@ -11947,13 +11954,13 @@
     </row>
     <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283" s="41" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B283" s="42"/>
       <c r="C283" s="42"/>
       <c r="D283" s="42"/>
       <c r="E283" s="42" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F283" s="43" t="s">
         <v>90</v>
@@ -11983,13 +11990,13 @@
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284" s="41" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B284" s="42"/>
       <c r="C284" s="42"/>
       <c r="D284" s="42"/>
       <c r="E284" s="42" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F284" s="43" t="s">
         <v>90</v>
@@ -12015,13 +12022,13 @@
     </row>
     <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285" s="41" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B285" s="42"/>
       <c r="C285" s="42"/>
       <c r="D285" s="42"/>
       <c r="E285" s="42" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F285" s="43" t="s">
         <v>90</v>
@@ -12045,13 +12052,13 @@
     </row>
     <row r="286" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A286" s="41" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B286" s="42"/>
       <c r="C286" s="42"/>
       <c r="D286" s="42"/>
       <c r="E286" s="42" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F286" s="43" t="s">
         <v>90</v>
@@ -12086,7 +12093,7 @@
       <c r="B287" s="56"/>
       <c r="C287" s="56"/>
       <c r="D287" s="56" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E287" s="56"/>
       <c r="F287" s="57" t="s">
@@ -12111,11 +12118,11 @@
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A288" s="30" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B288" s="63"/>
       <c r="C288" s="63" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D288" s="63"/>
       <c r="E288" s="63"/>
@@ -12152,7 +12159,7 @@
       <c r="B289" s="112"/>
       <c r="C289" s="42"/>
       <c r="D289" s="42" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E289" s="42"/>
       <c r="F289" s="43" t="s">
@@ -12184,7 +12191,7 @@
       <c r="B290" s="112"/>
       <c r="C290" s="42"/>
       <c r="D290" s="42" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E290" s="42"/>
       <c r="F290" s="43" t="s">
@@ -12220,7 +12227,7 @@
       <c r="B291" s="112"/>
       <c r="C291" s="42"/>
       <c r="D291" s="42" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E291" s="42"/>
       <c r="F291" s="43" t="s">
@@ -12252,7 +12259,7 @@
       <c r="B292" s="112"/>
       <c r="C292" s="42"/>
       <c r="D292" s="42" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E292" s="42"/>
       <c r="F292" s="43" t="s">
@@ -12284,7 +12291,7 @@
       <c r="B293" s="112"/>
       <c r="C293" s="42"/>
       <c r="D293" s="42" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E293" s="42"/>
       <c r="F293" s="43" t="s">
@@ -12318,7 +12325,7 @@
       <c r="B294" s="112"/>
       <c r="C294" s="42"/>
       <c r="D294" s="42" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E294" s="42"/>
       <c r="F294" s="43" t="s">
@@ -12352,7 +12359,7 @@
       <c r="B295" s="113"/>
       <c r="C295" s="56"/>
       <c r="D295" s="56" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E295" s="56"/>
       <c r="F295" s="57" t="s">
@@ -12379,11 +12386,11 @@
     </row>
     <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296" s="30" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B296" s="63"/>
       <c r="C296" s="63" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D296" s="63"/>
       <c r="E296" s="63"/>
@@ -12416,7 +12423,7 @@
       <c r="B297" s="112"/>
       <c r="C297" s="42"/>
       <c r="D297" s="42" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E297" s="42"/>
       <c r="F297" s="43" t="s">
@@ -12452,7 +12459,7 @@
       <c r="B298" s="112"/>
       <c r="C298" s="42"/>
       <c r="D298" s="42" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E298" s="42"/>
       <c r="F298" s="43" t="s">
@@ -12488,7 +12495,7 @@
       <c r="B299" s="112"/>
       <c r="C299" s="42"/>
       <c r="D299" s="42" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E299" s="42"/>
       <c r="F299" s="43" t="s">
@@ -12520,7 +12527,7 @@
       <c r="B300" s="112"/>
       <c r="C300" s="42"/>
       <c r="D300" s="42" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E300" s="42"/>
       <c r="F300" s="43" t="s">
@@ -12554,7 +12561,7 @@
       <c r="B301" s="112"/>
       <c r="C301" s="42"/>
       <c r="D301" s="42" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E301" s="42"/>
       <c r="F301" s="43" t="s">
@@ -12590,7 +12597,7 @@
       <c r="B302" s="42"/>
       <c r="C302" s="42"/>
       <c r="D302" s="42" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E302" s="42"/>
       <c r="F302" s="43" t="s">
@@ -12622,7 +12629,7 @@
       <c r="B303" s="56"/>
       <c r="C303" s="56"/>
       <c r="D303" s="56" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E303" s="56"/>
       <c r="F303" s="57" t="s">
@@ -12649,12 +12656,12 @@
     </row>
     <row r="304" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A304" s="41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B304" s="42"/>
       <c r="C304" s="42"/>
       <c r="D304" s="42" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E304" s="42"/>
       <c r="F304" s="43" t="s">
@@ -12685,13 +12692,13 @@
     </row>
     <row r="305" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A305" s="41" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B305" s="42"/>
       <c r="C305" s="42"/>
       <c r="D305" s="42"/>
       <c r="E305" s="42" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F305" s="43" t="s">
         <v>90</v>
@@ -12721,13 +12728,13 @@
     </row>
     <row r="306" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A306" s="41" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B306" s="42"/>
       <c r="C306" s="42"/>
       <c r="D306" s="42"/>
       <c r="E306" s="42" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F306" s="43" t="s">
         <v>90</v>
@@ -12755,12 +12762,12 @@
     </row>
     <row r="307" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A307" s="41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B307" s="42"/>
       <c r="C307" s="42"/>
       <c r="D307" s="42" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E307" s="42"/>
       <c r="F307" s="43" t="s">
@@ -12791,13 +12798,13 @@
     </row>
     <row r="308" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A308" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B308" s="42"/>
       <c r="C308" s="42"/>
       <c r="D308" s="42"/>
       <c r="E308" s="42" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F308" s="43" t="s">
         <v>90</v>
@@ -12823,13 +12830,13 @@
     </row>
     <row r="309" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A309" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B309" s="42"/>
       <c r="C309" s="42"/>
       <c r="D309" s="42"/>
       <c r="E309" s="42" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F309" s="43" t="s">
         <v>90</v>
@@ -12859,13 +12866,13 @@
     </row>
     <row r="310" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A310" s="41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B310" s="42"/>
       <c r="C310" s="42"/>
       <c r="D310" s="42"/>
       <c r="E310" s="42" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F310" s="43" t="s">
         <v>90</v>
@@ -12894,7 +12901,7 @@
       <c r="B311" s="42"/>
       <c r="C311" s="42"/>
       <c r="D311" s="42" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E311" s="42"/>
       <c r="F311" s="43" t="s">
@@ -12930,7 +12937,7 @@
       <c r="B312" s="42"/>
       <c r="C312" s="42"/>
       <c r="D312" s="42" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E312" s="42"/>
       <c r="F312" s="43" t="s">
@@ -12960,7 +12967,7 @@
       <c r="B313" s="42"/>
       <c r="C313" s="42"/>
       <c r="D313" s="42" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E313" s="42"/>
       <c r="F313" s="43" t="s">
@@ -12991,12 +12998,12 @@
     </row>
     <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314" s="41" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B314" s="42"/>
       <c r="C314" s="42"/>
       <c r="D314" s="42" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E314" s="42"/>
       <c r="F314" s="43" t="s">
@@ -13027,13 +13034,13 @@
     </row>
     <row r="315" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A315" s="41" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B315" s="42"/>
       <c r="C315" s="42"/>
       <c r="D315" s="42"/>
       <c r="E315" s="42" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F315" s="43" t="s">
         <v>29</v>
@@ -13063,13 +13070,13 @@
     </row>
     <row r="316" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A316" s="41" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B316" s="42"/>
       <c r="C316" s="42"/>
       <c r="D316" s="42"/>
       <c r="E316" s="42" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F316" s="43" t="s">
         <v>29</v>
@@ -13093,13 +13100,13 @@
     </row>
     <row r="317" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A317" s="41" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B317" s="42"/>
       <c r="C317" s="42"/>
       <c r="D317" s="42"/>
       <c r="E317" s="42" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F317" s="43" t="s">
         <v>29</v>
@@ -13126,7 +13133,7 @@
         <v>334</v>
       </c>
       <c r="D318" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F318" s="13" t="s">
         <v>90</v>
@@ -13157,7 +13164,7 @@
       <c r="B319" s="73"/>
       <c r="C319" s="73"/>
       <c r="D319" s="73" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E319" s="73"/>
       <c r="F319" s="57" t="s">
@@ -13192,7 +13199,7 @@
       </c>
       <c r="B320" s="31"/>
       <c r="C320" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D320" s="31"/>
       <c r="E320" s="31"/>
@@ -13229,7 +13236,7 @@
       <c r="B321" s="42"/>
       <c r="C321" s="42"/>
       <c r="D321" s="42" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E321" s="42"/>
       <c r="F321" s="43" t="s">
@@ -13261,7 +13268,7 @@
       <c r="B322" s="42"/>
       <c r="C322" s="42"/>
       <c r="D322" s="42" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E322" s="42"/>
       <c r="F322" s="43" t="s">
@@ -13293,7 +13300,7 @@
       <c r="B323" s="42"/>
       <c r="C323" s="42"/>
       <c r="D323" s="42" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E323" s="42"/>
       <c r="F323" s="43" t="s">
@@ -13327,7 +13334,7 @@
         <v>344</v>
       </c>
       <c r="D324" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F324" s="57" t="s">
         <v>29</v>
@@ -13357,11 +13364,11 @@
     </row>
     <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325" s="30" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B325" s="63"/>
       <c r="C325" s="63" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D325" s="63"/>
       <c r="E325" s="63"/>
@@ -13398,7 +13405,7 @@
       <c r="B326" s="42"/>
       <c r="C326" s="42"/>
       <c r="D326" s="42" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E326" s="42"/>
       <c r="F326" s="43" t="s">
@@ -13434,7 +13441,7 @@
       <c r="B327" s="42"/>
       <c r="C327" s="42"/>
       <c r="D327" s="42" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E327" s="42"/>
       <c r="F327" s="43" t="s">
@@ -13466,7 +13473,7 @@
       <c r="B328" s="42"/>
       <c r="C328" s="42"/>
       <c r="D328" s="42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E328" s="42"/>
       <c r="F328" s="43" t="s">
@@ -13493,12 +13500,12 @@
     </row>
     <row r="329" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A329" s="41" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B329" s="42"/>
       <c r="C329" s="42"/>
       <c r="D329" s="42" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E329" s="42"/>
       <c r="F329" s="43" t="s">
@@ -13523,13 +13530,13 @@
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A330" s="41" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B330" s="42"/>
       <c r="C330" s="42"/>
       <c r="D330" s="42"/>
       <c r="E330" s="42" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F330" s="43" t="s">
         <v>90</v>
@@ -13553,13 +13560,13 @@
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A331" s="41" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B331" s="42"/>
       <c r="C331" s="42"/>
       <c r="D331" s="42"/>
       <c r="E331" s="42" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F331" s="43" t="s">
         <v>90</v>
@@ -13588,7 +13595,7 @@
       <c r="B332" s="42"/>
       <c r="C332" s="42"/>
       <c r="D332" s="42" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E332" s="42"/>
       <c r="F332" s="43" t="s">
@@ -13620,7 +13627,7 @@
       <c r="B333" s="56"/>
       <c r="C333" s="56"/>
       <c r="D333" s="56" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E333" s="56"/>
       <c r="F333" s="57" t="s">
@@ -13649,11 +13656,11 @@
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A334" s="30" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B334" s="68"/>
       <c r="C334" s="68" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D334" s="68"/>
       <c r="E334" s="68"/>
@@ -13690,7 +13697,7 @@
       <c r="B335" s="42"/>
       <c r="C335" s="42"/>
       <c r="D335" s="42" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E335" s="42"/>
       <c r="F335" s="43" t="s">
@@ -13726,7 +13733,7 @@
       <c r="B336" s="42"/>
       <c r="C336" s="42"/>
       <c r="D336" s="42" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E336" s="42"/>
       <c r="F336" s="43" t="s">
@@ -13760,7 +13767,7 @@
       <c r="B337" s="42"/>
       <c r="C337" s="42"/>
       <c r="D337" s="42" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E337" s="42"/>
       <c r="F337" s="43" t="s">
@@ -13785,12 +13792,12 @@
     </row>
     <row r="338" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A338" s="41" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B338" s="42"/>
       <c r="C338" s="42"/>
       <c r="D338" s="42" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E338" s="42"/>
       <c r="F338" s="43" t="s">
@@ -13817,13 +13824,13 @@
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339" s="41" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B339" s="42"/>
       <c r="C339" s="42"/>
       <c r="D339" s="42"/>
       <c r="E339" s="42" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F339" s="43" t="s">
         <v>29</v>
@@ -13849,13 +13856,13 @@
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340" s="41" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B340" s="42"/>
       <c r="C340" s="42"/>
       <c r="D340" s="42"/>
       <c r="E340" s="42" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F340" s="43" t="s">
         <v>29</v>
@@ -13886,7 +13893,7 @@
       <c r="B341" s="42"/>
       <c r="C341" s="42"/>
       <c r="D341" s="42" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E341" s="42"/>
       <c r="F341" s="43" t="s">
@@ -13920,7 +13927,7 @@
       <c r="B342" s="42"/>
       <c r="C342" s="42"/>
       <c r="D342" s="42" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E342" s="42"/>
       <c r="F342" s="43" t="s">
@@ -13950,7 +13957,7 @@
       <c r="B343" s="42"/>
       <c r="C343" s="42"/>
       <c r="D343" s="42" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E343" s="42"/>
       <c r="F343" s="43" t="s">
@@ -13982,7 +13989,7 @@
       <c r="B344" s="94"/>
       <c r="C344" s="94"/>
       <c r="D344" s="94" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E344" s="94"/>
       <c r="F344" s="80" t="s">
@@ -14012,7 +14019,7 @@
       <c r="B345" s="73"/>
       <c r="C345" s="73"/>
       <c r="D345" s="73" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E345" s="73"/>
       <c r="F345" s="57" t="s">
@@ -14039,7 +14046,7 @@
     </row>
     <row r="346" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A346" s="117" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F346" s="13"/>
       <c r="G346" s="118"/>
@@ -14048,7 +14055,7 @@
     </row>
     <row r="347" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A347" s="117" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F347" s="13"/>
       <c r="G347" s="118"/>
@@ -14057,7 +14064,7 @@
     </row>
     <row r="348" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A348" s="117" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F348" s="13"/>
       <c r="G348" s="118"/>
@@ -14066,7 +14073,7 @@
     </row>
     <row r="349" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A349" s="117" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F349" s="13"/>
       <c r="G349" s="118"/>
@@ -14075,7 +14082,7 @@
     </row>
     <row r="350" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A350" s="117" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F350" s="13"/>
       <c r="G350" s="12"/>
@@ -14084,7 +14091,7 @@
     </row>
     <row r="351" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A351" s="117" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F351" s="13"/>
       <c r="G351" s="118"/>
@@ -14093,7 +14100,7 @@
     </row>
     <row r="352" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A352" s="117" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F352" s="13"/>
       <c r="G352" s="118"/>
@@ -14102,7 +14109,7 @@
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A353" s="117" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F353" s="13"/>
       <c r="G353" s="12"/>
@@ -14111,7 +14118,7 @@
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A354" s="117" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F354" s="13"/>
       <c r="G354" s="118"/>
@@ -14120,7 +14127,7 @@
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A355" s="117" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F355" s="13"/>
       <c r="G355" s="118"/>
@@ -14129,7 +14136,7 @@
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A356" s="117" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F356" s="13"/>
       <c r="K356" s="13"/>

</xml_diff>